<commit_message>
fix import export bantuan
</commit_message>
<xml_diff>
--- a/public/template/Template Impor Bantuan.xlsx
+++ b/public/template/Template Impor Bantuan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\kopaja\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35496994-9AC1-455A-A8D6-42FFFDBE9EE8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FF1B5E-95D9-427E-A51F-23BEE484DCA1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9812BD8F-7B10-4053-ACDF-F2695D87EBDE}"/>
+    <workbookView xWindow="4095" yWindow="1605" windowWidth="15375" windowHeight="7875" xr2:uid="{9812BD8F-7B10-4053-ACDF-F2695D87EBDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,16 +36,16 @@
     <t>NO</t>
   </si>
   <si>
-    <t>PERTANYAAN</t>
-  </si>
-  <si>
-    <t>JAWABAN</t>
-  </si>
-  <si>
     <t>Apa itu kopaja.id?</t>
   </si>
   <si>
     <t>Kopaja.id adalah sebuah website belajar perpajakan online yang kami sediakan bagi siswa-siswi SMA/SMK</t>
+  </si>
+  <si>
+    <t>QUESTION</t>
+  </si>
+  <si>
+    <t>ANSWER</t>
   </si>
 </sst>
 </file>
@@ -473,7 +473,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -494,10 +494,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -510,10 +510,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -526,10 +526,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -542,10 +542,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="10"/>
@@ -558,10 +558,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -574,10 +574,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>

</xml_diff>